<commit_message>
boitier--> medecin (vassort, pellat)
</commit_message>
<xml_diff>
--- a/results/AMPLI-CATEGORY/2021_stats.xlsx
+++ b/results/AMPLI-CATEGORY/2021_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="42">
   <si>
     <t>Annee</t>
   </si>
@@ -100,12 +100,15 @@
     <t>Vasculaire - Angiographie</t>
   </si>
   <si>
-    <t>Cardiologie</t>
+    <t>Cardio-Rythmologie</t>
   </si>
   <si>
     <t>Vasculaire - Abdo Angioplastie simple</t>
   </si>
   <si>
+    <t>Vasculaire - Abdo Angioplastie complexe</t>
+  </si>
+  <si>
     <t>Cardio- Coro + Angioplastie complexe (&gt;1vx)</t>
   </si>
   <si>
@@ -127,13 +130,7 @@
     <t>Douleur</t>
   </si>
   <si>
-    <t>Vasculaire - Abdo Angioplastie complexe</t>
-  </si>
-  <si>
     <t>Cardio-CTO</t>
-  </si>
-  <si>
-    <t>Cardio-Rythmologie</t>
   </si>
   <si>
     <t>Cardio- Angioplastie simple (=1vx)</t>
@@ -500,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -886,22 +883,25 @@
         <v>28</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13">
-        <v>3.739</v>
+        <v>3.645</v>
       </c>
       <c r="G13">
-        <v>5.435</v>
+        <v>5.369</v>
       </c>
       <c r="H13">
-        <v>2.321</v>
+        <v>1.75</v>
       </c>
       <c r="I13">
-        <v>96</v>
+        <v>51</v>
+      </c>
+      <c r="J13">
+        <v>63.64</v>
       </c>
       <c r="K13">
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -950,28 +950,28 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E15">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F15">
-        <v>169.404</v>
+        <v>153.38</v>
       </c>
       <c r="G15">
-        <v>168.489</v>
+        <v>165.93</v>
       </c>
       <c r="H15">
-        <v>117.042</v>
+        <v>106.69</v>
       </c>
       <c r="I15">
-        <v>1465.774</v>
+        <v>1340</v>
       </c>
       <c r="J15">
-        <v>1076.672</v>
+        <v>1078.175</v>
       </c>
       <c r="K15">
-        <v>1029</v>
+        <v>986</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1046,7 +1046,7 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E18">
         <v>27</v>
@@ -1081,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -1142,7 +1142,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -1177,7 +1177,7 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22">
         <v>9</v>
@@ -1212,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1276,28 +1276,28 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F25">
-        <v>18.774</v>
+        <v>50.279</v>
       </c>
       <c r="G25">
-        <v>17.369</v>
+        <v>29.046</v>
       </c>
       <c r="H25">
-        <v>15.984</v>
+        <v>57.145</v>
       </c>
       <c r="I25">
-        <v>365.25</v>
+        <v>981.7140000000001</v>
       </c>
       <c r="J25">
-        <v>389.893</v>
+        <v>496.054</v>
       </c>
       <c r="K25">
-        <v>186</v>
+        <v>985</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1311,28 +1311,22 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>50.279</v>
-      </c>
-      <c r="G26">
-        <v>29.046</v>
+        <v>1.414</v>
       </c>
       <c r="H26">
-        <v>57.145</v>
+        <v>1.414</v>
       </c>
       <c r="I26">
-        <v>981.7140000000001</v>
-      </c>
-      <c r="J26">
-        <v>496.054</v>
+        <v>77</v>
       </c>
       <c r="K26">
-        <v>985</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1346,22 +1340,28 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27">
-        <v>1.414</v>
+        <v>19.578</v>
+      </c>
+      <c r="G27">
+        <v>10.308</v>
       </c>
       <c r="H27">
-        <v>1.414</v>
+        <v>19.578</v>
       </c>
       <c r="I27">
-        <v>77</v>
+        <v>300</v>
+      </c>
+      <c r="J27">
+        <v>82.024</v>
       </c>
       <c r="K27">
-        <v>77</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1375,22 +1375,22 @@
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>0.8179999999999999</v>
+        <v>4.81</v>
       </c>
       <c r="H28">
-        <v>0.8179999999999999</v>
+        <v>4.81</v>
       </c>
       <c r="I28">
-        <v>6</v>
+        <v>424</v>
       </c>
       <c r="K28">
-        <v>6</v>
+        <v>424</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1401,31 +1401,31 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="F29">
-        <v>19.578</v>
+        <v>17.341</v>
       </c>
       <c r="G29">
-        <v>10.308</v>
+        <v>15.598</v>
       </c>
       <c r="H29">
-        <v>19.578</v>
+        <v>12.434</v>
       </c>
       <c r="I29">
-        <v>300</v>
+        <v>346.559</v>
       </c>
       <c r="J29">
-        <v>82.024</v>
+        <v>320.181</v>
       </c>
       <c r="K29">
-        <v>300</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1436,25 +1436,31 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>713</v>
       </c>
       <c r="F30">
-        <v>4.81</v>
+        <v>27.26</v>
+      </c>
+      <c r="G30">
+        <v>18.845</v>
       </c>
       <c r="H30">
-        <v>4.81</v>
+        <v>21.908</v>
       </c>
       <c r="I30">
-        <v>424</v>
+        <v>643.98</v>
+      </c>
+      <c r="J30">
+        <v>435.352</v>
       </c>
       <c r="K30">
-        <v>424</v>
+        <v>516</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1468,28 +1474,28 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E31">
-        <v>774</v>
+        <v>63</v>
       </c>
       <c r="F31">
-        <v>17.341</v>
+        <v>58.789</v>
       </c>
       <c r="G31">
-        <v>15.598</v>
+        <v>41.789</v>
       </c>
       <c r="H31">
-        <v>12.434</v>
+        <v>44.826</v>
       </c>
       <c r="I31">
-        <v>346.559</v>
+        <v>1818.778</v>
       </c>
       <c r="J31">
-        <v>320.181</v>
+        <v>1154.669</v>
       </c>
       <c r="K31">
-        <v>242</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1503,28 +1509,28 @@
         <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E32">
-        <v>713</v>
+        <v>4</v>
       </c>
       <c r="F32">
-        <v>27.26</v>
+        <v>40.49</v>
       </c>
       <c r="G32">
-        <v>18.845</v>
+        <v>16.199</v>
       </c>
       <c r="H32">
-        <v>21.908</v>
+        <v>45.357</v>
       </c>
       <c r="I32">
-        <v>643.98</v>
+        <v>1040.25</v>
       </c>
       <c r="J32">
-        <v>435.352</v>
+        <v>330.67</v>
       </c>
       <c r="K32">
-        <v>516</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1538,28 +1544,28 @@
         <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E33">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="F33">
-        <v>58.789</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="G33">
-        <v>41.789</v>
+        <v>1.029</v>
       </c>
       <c r="H33">
-        <v>44.826</v>
+        <v>0.275</v>
       </c>
       <c r="I33">
-        <v>1818.778</v>
+        <v>23.25</v>
       </c>
       <c r="J33">
-        <v>1154.669</v>
+        <v>25.194</v>
       </c>
       <c r="K33">
-        <v>1613</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1573,28 +1579,28 @@
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F34">
-        <v>40.49</v>
+        <v>37.38</v>
       </c>
       <c r="G34">
-        <v>16.199</v>
+        <v>24.216</v>
       </c>
       <c r="H34">
-        <v>45.357</v>
+        <v>31.157</v>
       </c>
       <c r="I34">
-        <v>1040.25</v>
+        <v>1044.833</v>
       </c>
       <c r="J34">
-        <v>330.67</v>
+        <v>656.076</v>
       </c>
       <c r="K34">
-        <v>1095</v>
+        <v>924.5</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1608,28 +1614,28 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E35">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F35">
-        <v>0.8149999999999999</v>
+        <v>14.472</v>
       </c>
       <c r="G35">
-        <v>1.029</v>
+        <v>15.462</v>
       </c>
       <c r="H35">
-        <v>0.275</v>
+        <v>9.387</v>
       </c>
       <c r="I35">
-        <v>23.25</v>
+        <v>473</v>
       </c>
       <c r="J35">
-        <v>25.194</v>
+        <v>469.266</v>
       </c>
       <c r="K35">
-        <v>15.5</v>
+        <v>293.5</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1643,28 +1649,28 @@
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E36">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F36">
-        <v>37.38</v>
+        <v>64.673</v>
       </c>
       <c r="G36">
-        <v>24.216</v>
+        <v>55.416</v>
       </c>
       <c r="H36">
-        <v>31.157</v>
+        <v>64.673</v>
       </c>
       <c r="I36">
-        <v>1044.833</v>
+        <v>1066</v>
       </c>
       <c r="J36">
-        <v>656.076</v>
+        <v>120.208</v>
       </c>
       <c r="K36">
-        <v>924.5</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1678,28 +1684,28 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E37">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>14.472</v>
+        <v>3.559</v>
       </c>
       <c r="G37">
-        <v>15.462</v>
+        <v>2.633</v>
       </c>
       <c r="H37">
-        <v>9.387</v>
+        <v>3.559</v>
       </c>
       <c r="I37">
-        <v>473</v>
+        <v>359.5</v>
       </c>
       <c r="J37">
-        <v>469.266</v>
+        <v>395.273</v>
       </c>
       <c r="K37">
-        <v>293.5</v>
+        <v>359.5</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1713,28 +1719,22 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <v>64.673</v>
-      </c>
-      <c r="G38">
-        <v>55.416</v>
+        <v>4.069</v>
       </c>
       <c r="H38">
-        <v>64.673</v>
+        <v>4.069</v>
       </c>
       <c r="I38">
-        <v>1066</v>
-      </c>
-      <c r="J38">
-        <v>120.208</v>
+        <v>114</v>
       </c>
       <c r="K38">
-        <v>1066</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1745,31 +1745,31 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>242</v>
       </c>
       <c r="F39">
-        <v>3.559</v>
+        <v>3.389</v>
       </c>
       <c r="G39">
-        <v>2.633</v>
+        <v>3.88</v>
       </c>
       <c r="H39">
-        <v>3.559</v>
+        <v>2.404</v>
       </c>
       <c r="I39">
-        <v>359.5</v>
+        <v>78</v>
       </c>
       <c r="J39">
-        <v>395.273</v>
+        <v>79.07599999999999</v>
       </c>
       <c r="K39">
-        <v>359.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1780,25 +1780,22 @@
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F40">
-        <v>4.069</v>
+        <v>2.554</v>
+      </c>
+      <c r="G40">
+        <v>2.82</v>
       </c>
       <c r="H40">
-        <v>4.069</v>
-      </c>
-      <c r="I40">
-        <v>114</v>
-      </c>
-      <c r="K40">
-        <v>114</v>
+        <v>1.394</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1812,28 +1809,16 @@
         <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E41">
-        <v>242</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>3.389</v>
-      </c>
-      <c r="G41">
-        <v>3.88</v>
+        <v>4.699</v>
       </c>
       <c r="H41">
-        <v>2.404</v>
-      </c>
-      <c r="I41">
-        <v>78</v>
-      </c>
-      <c r="J41">
-        <v>79.07599999999999</v>
-      </c>
-      <c r="K41">
-        <v>74</v>
+        <v>4.699</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1847,19 +1832,19 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E42">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F42">
-        <v>2.554</v>
+        <v>6.428</v>
       </c>
       <c r="G42">
-        <v>2.82</v>
+        <v>8.148999999999999</v>
       </c>
       <c r="H42">
-        <v>1.394</v>
+        <v>6.428</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1873,16 +1858,16 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
-        <v>4.699</v>
+        <v>0.38</v>
       </c>
       <c r="H43">
-        <v>4.699</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1893,22 +1878,22 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>585</v>
       </c>
       <c r="F44">
-        <v>6.428</v>
+        <v>1.143</v>
       </c>
       <c r="G44">
-        <v>8.148999999999999</v>
+        <v>3.567</v>
       </c>
       <c r="H44">
-        <v>6.428</v>
+        <v>0.236</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -1919,19 +1904,31 @@
         <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="F45">
-        <v>0.38</v>
+        <v>1.509</v>
+      </c>
+      <c r="G45">
+        <v>4.355</v>
       </c>
       <c r="H45">
-        <v>0.38</v>
+        <v>0.484</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -1945,19 +1942,19 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E46">
-        <v>585</v>
+        <v>13</v>
       </c>
       <c r="F46">
-        <v>1.143</v>
+        <v>1.426</v>
       </c>
       <c r="G46">
-        <v>3.567</v>
+        <v>1.225</v>
       </c>
       <c r="H46">
-        <v>0.236</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -1971,28 +1968,19 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E47">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="F47">
-        <v>1.509</v>
+        <v>1.151</v>
       </c>
       <c r="G47">
-        <v>4.355</v>
+        <v>0.949</v>
       </c>
       <c r="H47">
-        <v>0.484</v>
-      </c>
-      <c r="I47">
-        <v>3</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>3</v>
+        <v>0.8179999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2006,19 +1994,19 @@
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E48">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F48">
-        <v>1.426</v>
+        <v>1.573</v>
       </c>
       <c r="G48">
-        <v>1.225</v>
+        <v>1.615</v>
       </c>
       <c r="H48">
-        <v>0.71</v>
+        <v>1.497</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2032,19 +2020,19 @@
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E49">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F49">
-        <v>1.151</v>
+        <v>0.646</v>
       </c>
       <c r="G49">
-        <v>0.949</v>
+        <v>0.519</v>
       </c>
       <c r="H49">
-        <v>0.8179999999999999</v>
+        <v>0.522</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2058,19 +2046,19 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E50">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F50">
-        <v>1.573</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="G50">
-        <v>1.615</v>
+        <v>0.096</v>
       </c>
       <c r="H50">
-        <v>1.497</v>
+        <v>0.08599999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2081,22 +2069,31 @@
         <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="F51">
-        <v>0.646</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G51">
-        <v>0.519</v>
+        <v>0.038</v>
       </c>
       <c r="H51">
-        <v>0.522</v>
+        <v>0.001</v>
+      </c>
+      <c r="I51">
+        <v>2.667</v>
+      </c>
+      <c r="J51">
+        <v>2.887</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2107,22 +2104,28 @@
         <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="F52">
-        <v>0.08599999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="G52">
-        <v>0.096</v>
+        <v>0.029</v>
       </c>
       <c r="H52">
-        <v>0.08599999999999999</v>
+        <v>0.003</v>
+      </c>
+      <c r="I52">
+        <v>9</v>
+      </c>
+      <c r="K52">
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2136,28 +2139,19 @@
         <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E53">
-        <v>452</v>
+        <v>2</v>
       </c>
       <c r="F53">
-        <v>0.008999999999999999</v>
+        <v>0.006</v>
       </c>
       <c r="G53">
-        <v>0.038</v>
+        <v>0.001</v>
       </c>
       <c r="H53">
-        <v>0.001</v>
-      </c>
-      <c r="I53">
-        <v>2.667</v>
-      </c>
-      <c r="J53">
-        <v>2.887</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2171,25 +2165,19 @@
         <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E54">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F54">
-        <v>0.015</v>
+        <v>0.024</v>
       </c>
       <c r="G54">
-        <v>0.029</v>
+        <v>0.014</v>
       </c>
       <c r="H54">
-        <v>0.003</v>
-      </c>
-      <c r="I54">
-        <v>9</v>
-      </c>
-      <c r="K54">
-        <v>9</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2200,22 +2188,31 @@
         <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="F55">
-        <v>0.006</v>
+        <v>0.259</v>
       </c>
       <c r="G55">
-        <v>0.001</v>
+        <v>0.488</v>
       </c>
       <c r="H55">
-        <v>0.006</v>
+        <v>0.105</v>
+      </c>
+      <c r="I55">
+        <v>30</v>
+      </c>
+      <c r="J55">
+        <v>16.971</v>
+      </c>
+      <c r="K55">
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2226,22 +2223,22 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>197</v>
       </c>
       <c r="F56">
-        <v>0.024</v>
+        <v>0.126</v>
       </c>
       <c r="G56">
-        <v>0.014</v>
+        <v>0.196</v>
       </c>
       <c r="H56">
-        <v>0.024</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2255,28 +2252,19 @@
         <v>17</v>
       </c>
       <c r="D57" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E57">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="F57">
-        <v>0.259</v>
+        <v>0.131</v>
       </c>
       <c r="G57">
-        <v>0.488</v>
+        <v>0.082</v>
       </c>
       <c r="H57">
         <v>0.105</v>
-      </c>
-      <c r="I57">
-        <v>30</v>
-      </c>
-      <c r="J57">
-        <v>16.971</v>
-      </c>
-      <c r="K57">
-        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2290,19 +2278,25 @@
         <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E58">
-        <v>197</v>
+        <v>12</v>
       </c>
       <c r="F58">
-        <v>0.126</v>
+        <v>8.804</v>
       </c>
       <c r="G58">
-        <v>0.196</v>
+        <v>8.741</v>
       </c>
       <c r="H58">
-        <v>0.055</v>
+        <v>5.479</v>
+      </c>
+      <c r="I58">
+        <v>330</v>
+      </c>
+      <c r="K58">
+        <v>330</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2316,19 +2310,28 @@
         <v>17</v>
       </c>
       <c r="D59" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E59">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="F59">
-        <v>0.131</v>
+        <v>1.796</v>
       </c>
       <c r="G59">
-        <v>0.082</v>
+        <v>6.921</v>
       </c>
       <c r="H59">
-        <v>0.105</v>
+        <v>0.359</v>
+      </c>
+      <c r="I59">
+        <v>446.5</v>
+      </c>
+      <c r="J59">
+        <v>309.006</v>
+      </c>
+      <c r="K59">
+        <v>446.5</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2342,28 +2345,28 @@
         <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E60">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F60">
-        <v>10.227</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>15.621</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>4.917</v>
+        <v>0</v>
       </c>
       <c r="I60">
-        <v>497.5</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>236.881</v>
+        <v>0</v>
       </c>
       <c r="K60">
-        <v>497.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2377,25 +2380,19 @@
         <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E61">
-        <v>98</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>1.105</v>
+        <v>2.434</v>
       </c>
       <c r="G61">
-        <v>3.027</v>
+        <v>3.489</v>
       </c>
       <c r="H61">
-        <v>0.354</v>
-      </c>
-      <c r="I61">
-        <v>228</v>
-      </c>
-      <c r="K61">
-        <v>228</v>
+        <v>1.123</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2409,24 +2406,18 @@
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
       <c r="H62">
         <v>0</v>
       </c>
       <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
         <v>0</v>
       </c>
       <c r="K62">
@@ -2441,22 +2432,28 @@
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D63" t="s">
         <v>19</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F63">
-        <v>2.434</v>
+        <v>9.06</v>
       </c>
       <c r="G63">
-        <v>3.489</v>
+        <v>10.999</v>
       </c>
       <c r="H63">
-        <v>1.123</v>
+        <v>6.495</v>
+      </c>
+      <c r="I63">
+        <v>90</v>
+      </c>
+      <c r="K63">
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2467,79 +2464,18 @@
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>1.109</v>
       </c>
       <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65">
-        <v>80</v>
-      </c>
-      <c r="F65">
-        <v>9.06</v>
-      </c>
-      <c r="G65">
-        <v>10.999</v>
-      </c>
-      <c r="H65">
-        <v>6.495</v>
-      </c>
-      <c r="I65">
-        <v>90</v>
-      </c>
-      <c r="K65">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66" t="s">
-        <v>22</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66">
-        <v>1.109</v>
-      </c>
-      <c r="H66">
         <v>1.109</v>
       </c>
     </row>

</xml_diff>